<commit_message>
Projeto Traders: Em Desenvolvimento Projeto Algoritmos: Desenvolvimento dos calculos dos produtos unitários.
</commit_message>
<xml_diff>
--- a/Projeto Traders/Projeto Algoritmos/Calcular Dolar e Indice.xlsx
+++ b/Projeto Traders/Projeto Algoritmos/Calcular Dolar e Indice.xlsx
@@ -1,48 +1,470 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiexin\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24975" windowHeight="10155"/>
+    <workbookView windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Indice e Dólar" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
+  <si>
+    <t>Dados a inserir:</t>
+  </si>
+  <si>
+    <t>Ativo:</t>
+  </si>
+  <si>
+    <t>WIN</t>
+  </si>
+  <si>
+    <t>Contratos:</t>
+  </si>
+  <si>
+    <t>Dólar PTAX:</t>
+  </si>
+  <si>
+    <t>Configuração</t>
+  </si>
+  <si>
+    <t>Corretora:</t>
+  </si>
+  <si>
+    <t>Corretagem:</t>
+  </si>
+  <si>
+    <t>Taxa ISS:</t>
+  </si>
+  <si>
+    <t>Tarifas da Bolsa de Valores:</t>
+  </si>
+  <si>
+    <t>Insentivos:</t>
+  </si>
+  <si>
+    <t>Emolumentos:</t>
+  </si>
+  <si>
+    <t>Mini Contratos:</t>
+  </si>
+  <si>
+    <t>Taxa Registro Variável:</t>
+  </si>
+  <si>
+    <t>DayTrade</t>
+  </si>
+  <si>
+    <t>Taxa Registro Fixo:</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -50,24 +472,334 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="40% - Ênfase 4" xfId="3" builtinId="43"/>
+    <cellStyle name="Porcentagem" xfId="4" builtinId="5"/>
+    <cellStyle name="Célula Vinculada" xfId="5" builtinId="24"/>
+    <cellStyle name="Célula de Verificação" xfId="6" builtinId="23"/>
+    <cellStyle name="Moeda [0]" xfId="7" builtinId="7"/>
+    <cellStyle name="20% - Ênfase 3" xfId="8" builtinId="38"/>
+    <cellStyle name="Moeda" xfId="9" builtinId="4"/>
+    <cellStyle name="Hyperlink seguido" xfId="10" builtinId="9"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8"/>
+    <cellStyle name="40% - Ênfase 2" xfId="12" builtinId="35"/>
+    <cellStyle name="Observação" xfId="13" builtinId="10"/>
+    <cellStyle name="40% - Ênfase 6" xfId="14" builtinId="51"/>
+    <cellStyle name="Texto de Aviso" xfId="15" builtinId="11"/>
+    <cellStyle name="Título" xfId="16" builtinId="15"/>
+    <cellStyle name="Texto Explicativo" xfId="17" builtinId="53"/>
+    <cellStyle name="Ênfase 3" xfId="18" builtinId="37"/>
+    <cellStyle name="Título 1" xfId="19" builtinId="16"/>
+    <cellStyle name="Ênfase 4" xfId="20" builtinId="41"/>
+    <cellStyle name="Título 2" xfId="21" builtinId="17"/>
+    <cellStyle name="Ênfase 5" xfId="22" builtinId="45"/>
+    <cellStyle name="Título 3" xfId="23" builtinId="18"/>
+    <cellStyle name="Ênfase 6" xfId="24" builtinId="49"/>
+    <cellStyle name="Título 4" xfId="25" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="26" builtinId="20"/>
+    <cellStyle name="Saída" xfId="27" builtinId="21"/>
+    <cellStyle name="Cálculo" xfId="28" builtinId="22"/>
+    <cellStyle name="Total" xfId="29" builtinId="25"/>
+    <cellStyle name="40% - Ênfase 1" xfId="30" builtinId="31"/>
+    <cellStyle name="Bom" xfId="31" builtinId="26"/>
+    <cellStyle name="Ruim" xfId="32" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="33" builtinId="28"/>
+    <cellStyle name="20% - Ênfase 5" xfId="34" builtinId="46"/>
+    <cellStyle name="Ênfase 1" xfId="35" builtinId="29"/>
+    <cellStyle name="20% - Ênfase 1" xfId="36" builtinId="30"/>
+    <cellStyle name="60% - Ênfase 1" xfId="37" builtinId="32"/>
+    <cellStyle name="20% - Ênfase 6" xfId="38" builtinId="50"/>
+    <cellStyle name="Ênfase 2" xfId="39" builtinId="33"/>
+    <cellStyle name="20% - Ênfase 2" xfId="40" builtinId="34"/>
+    <cellStyle name="60% - Ênfase 2" xfId="41" builtinId="36"/>
+    <cellStyle name="40% - Ênfase 3" xfId="42" builtinId="39"/>
+    <cellStyle name="60% - Ênfase 3" xfId="43" builtinId="40"/>
+    <cellStyle name="20% - Ênfase 4" xfId="44" builtinId="42"/>
+    <cellStyle name="60% - Ênfase 4" xfId="45" builtinId="44"/>
+    <cellStyle name="40% - Ênfase 5" xfId="46" builtinId="47"/>
+    <cellStyle name="60% - Ênfase 5" xfId="47" builtinId="48"/>
+    <cellStyle name="60% - Ênfase 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -116,7 +848,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -151,7 +883,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,23 +1057,118 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="12.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="A15:B15"/>
+  </mergeCells>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Projeto Traders: Em Desenvolvimento. Projeto Algoritmos: informações adicionais.
custos operacionais no mini indice:

Taxa de registro BMF: R$0,08 cada mini (aproximadamente)
Emolumentos: R$0,05 cada mini (aproximadamente)
Iss/PIS/Cofins: 9,65% do valor da corretagem
</commit_message>
<xml_diff>
--- a/Projeto Traders/Projeto Algoritmos/Calcular Dolar e Indice.xlsx
+++ b/Projeto Traders/Projeto Algoritmos/Calcular Dolar e Indice.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57">
   <si>
     <t>Dados a inserir:</t>
   </si>
@@ -49,12 +49,21 @@
     <t>Configuração</t>
   </si>
   <si>
+    <t>aproximadamente</t>
+  </si>
+  <si>
     <t>Corretora:</t>
   </si>
   <si>
+    <t>Registro BMF:</t>
+  </si>
+  <si>
     <t>Corretagem:</t>
   </si>
   <si>
+    <t>Emolumentos:</t>
+  </si>
+  <si>
     <t>Taxa ISS:</t>
   </si>
   <si>
@@ -68,9 +77,6 @@
   </si>
   <si>
     <t>Insentivos:</t>
-  </si>
-  <si>
-    <t>Emolumentos:</t>
   </si>
   <si>
     <t>Mini Contratos:</t>
@@ -227,6 +233,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -234,7 +263,90 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,27 +368,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -286,96 +377,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="45">
     <fill>
@@ -464,181 +470,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,27 +688,30 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -747,15 +756,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -771,163 +771,169 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="39" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="42" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -938,6 +944,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1316,7 +1325,7 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1324,6 +1333,7 @@
     <col min="1" max="1" width="20.5714285714286" customWidth="1"/>
     <col min="2" max="2" width="15.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="12.8571428571429"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="10.1428571428571" customWidth="1"/>
     <col min="7" max="9" width="10.8571428571429" customWidth="1"/>
@@ -1351,7 +1361,7 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="L2" t="s">
@@ -1371,7 +1381,7 @@
       <c r="J3">
         <v>2</v>
       </c>
-      <c r="K3" s="25"/>
+      <c r="K3" s="26"/>
       <c r="L3">
         <v>1</v>
       </c>
@@ -1389,13 +1399,13 @@
       <c r="J4">
         <v>3</v>
       </c>
-      <c r="K4" s="25"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" spans="10:11">
       <c r="J5">
         <v>4</v>
       </c>
-      <c r="K5" s="25"/>
+      <c r="K5" s="26"/>
     </row>
     <row r="6" customHeight="1" spans="1:11">
       <c r="A6" t="s">
@@ -1404,386 +1414,402 @@
       <c r="J6">
         <v>5</v>
       </c>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="10:11">
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" spans="4:11">
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6"/>
       <c r="J7">
         <v>6</v>
       </c>
-      <c r="K7" s="20"/>
+      <c r="K7" s="21"/>
     </row>
     <row r="8" customHeight="1" spans="1:11">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>0.08</v>
       </c>
       <c r="J8">
         <v>7</v>
       </c>
-      <c r="K8" s="20"/>
+      <c r="K8" s="21"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="7">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="8">
         <v>0.09</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>0.05</v>
+      </c>
       <c r="J9">
         <v>8</v>
       </c>
-      <c r="K9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="7">
-        <v>9</v>
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="8">
+        <v>9.65</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J10">
         <v>9</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="10">
         <v>0</v>
       </c>
       <c r="J11">
         <v>10</v>
       </c>
-      <c r="K11" s="25"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="10:11">
       <c r="J12">
         <v>11</v>
       </c>
-      <c r="K12" s="25"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10" t="s">
+      <c r="A13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="F13" s="11"/>
       <c r="J13">
         <v>12</v>
       </c>
-      <c r="K13" s="25"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="7">
+      <c r="A14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="8">
         <f>(G39*B4)/F32</f>
         <v>0.91</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="7">
+      <c r="D14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="8">
         <v>0.21</v>
       </c>
       <c r="G14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J14">
         <v>13</v>
       </c>
-      <c r="K14" s="25"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13">
+      <c r="A15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14">
         <f>((G51*B4)/F44)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G15" t="s">
         <v>22</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G15" t="s">
-        <v>20</v>
       </c>
       <c r="J15">
         <v>14</v>
       </c>
-      <c r="K15" s="25"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13">
+      <c r="A16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14">
         <v>0.1166181</v>
       </c>
       <c r="J16">
         <v>15</v>
       </c>
-      <c r="K16" s="25"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17" spans="10:11">
       <c r="J17">
         <v>16</v>
       </c>
-      <c r="K17" s="25"/>
+      <c r="K17" s="26"/>
     </row>
     <row r="18" spans="10:11">
       <c r="J18">
         <v>17</v>
       </c>
-      <c r="K18" s="25"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J19">
         <v>18</v>
       </c>
-      <c r="K19" s="25"/>
+      <c r="K19" s="26"/>
     </row>
     <row r="20" spans="6:11">
       <c r="F20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
       <c r="J20">
         <v>19</v>
       </c>
-      <c r="K20" s="25"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I21" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J21">
         <v>20</v>
       </c>
-      <c r="K21" s="25"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16">
+      <c r="A22" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17">
         <f>B9*B3</f>
         <v>0.18</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18">
+      <c r="D22" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="19">
         <f>(C15*C16)*(F15)*(F14)</f>
         <v>0.0122449005</v>
       </c>
-      <c r="H22" s="19">
-        <v>0.01</v>
-      </c>
-      <c r="I22" s="18">
+      <c r="H22" s="20">
+        <v>0.09</v>
+      </c>
+      <c r="I22" s="19">
         <f>H22*B3</f>
-        <v>0.02</v>
+        <v>0.18</v>
       </c>
       <c r="J22">
         <v>21</v>
       </c>
-      <c r="K22" s="25"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="16">
+      <c r="A23" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17">
         <f>C22*(B10/100)</f>
-        <v>0.0162</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18">
+        <v>0.01737</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19">
         <f>(C14*(F15))*(F14)</f>
         <v>0.09555</v>
       </c>
-      <c r="H23" s="19">
-        <v>0.09</v>
-      </c>
-      <c r="I23" s="18">
+      <c r="H23" s="20">
+        <v>0.06</v>
+      </c>
+      <c r="I23" s="19">
         <f>H23*B3</f>
-        <v>0.18</v>
-      </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="20" t="s">
-        <v>35</v>
+        <v>0.12</v>
+      </c>
+      <c r="J23" s="27"/>
+      <c r="K23" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="L23">
         <f>SUM(L3:L22)</f>
         <v>1</v>
       </c>
-      <c r="M23" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="N23" s="27"/>
+      <c r="M23" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="N23" s="28"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="16">
+      <c r="A24" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17">
         <f>B11</f>
         <v>0</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18">
+      <c r="D24" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="19">
         <f>I22+I23</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="K24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L24">
         <f>L23/21</f>
         <v>0.0476190476190476</v>
       </c>
-      <c r="M24" s="27">
+      <c r="M24" s="28">
         <v>1</v>
       </c>
-      <c r="N24" s="27"/>
+      <c r="N24" s="28"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16">
+      <c r="A25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17">
         <f>C22+C23+C24</f>
-        <v>0.1962</v>
+        <v>0.19737</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <f>C25+G24</f>
-        <v>0.3962</v>
+        <v>0.49737</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>42</v>
+      <c r="B29" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="30" ht="15.75" spans="1:4">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" ht="15.75" spans="1:7">
-      <c r="A31" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21" t="s">
-        <v>46</v>
+      <c r="A31" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" ht="15.75" spans="1:7">
-      <c r="A32" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="22" t="s">
+      <c r="A32" s="23" t="s">
         <v>52</v>
       </c>
+      <c r="B32" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>54</v>
+      </c>
       <c r="D32" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F32">
         <f>M24</f>
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" ht="15.75" spans="1:7">
-      <c r="A33" s="23">
+      <c r="A33" s="24">
         <v>1</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="24">
         <v>10</v>
       </c>
-      <c r="C33" s="23">
+      <c r="C33" s="24">
         <v>0.91</v>
       </c>
       <c r="D33">
@@ -1800,13 +1826,13 @@
       </c>
     </row>
     <row r="34" ht="15.75" spans="1:7">
-      <c r="A34" s="23">
+      <c r="A34" s="24">
         <v>11</v>
       </c>
-      <c r="B34" s="23">
+      <c r="B34" s="24">
         <v>50</v>
       </c>
-      <c r="C34" s="23">
+      <c r="C34" s="24">
         <v>0.81</v>
       </c>
       <c r="D34">
@@ -1823,13 +1849,13 @@
       </c>
     </row>
     <row r="35" ht="15.75" spans="1:7">
-      <c r="A35" s="23">
+      <c r="A35" s="24">
         <v>51</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="24">
         <v>100</v>
       </c>
-      <c r="C35" s="23">
+      <c r="C35" s="24">
         <v>0.78</v>
       </c>
       <c r="D35">
@@ -1846,13 +1872,13 @@
       </c>
     </row>
     <row r="36" ht="15.75" spans="1:7">
-      <c r="A36" s="23">
+      <c r="A36" s="24">
         <v>101</v>
       </c>
-      <c r="B36" s="23">
+      <c r="B36" s="24">
         <v>190</v>
       </c>
-      <c r="C36" s="23">
+      <c r="C36" s="24">
         <v>0.73</v>
       </c>
       <c r="D36">
@@ -1869,13 +1895,13 @@
       </c>
     </row>
     <row r="37" ht="15.75" spans="1:7">
-      <c r="A37" s="23">
+      <c r="A37" s="24">
         <v>191</v>
       </c>
-      <c r="B37" s="23">
+      <c r="B37" s="24">
         <v>2000</v>
       </c>
-      <c r="C37" s="23">
+      <c r="C37" s="24">
         <v>0.68</v>
       </c>
       <c r="D37">
@@ -1892,11 +1918,11 @@
       </c>
     </row>
     <row r="38" ht="15.75" spans="1:7">
-      <c r="A38" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23">
+      <c r="A38" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24">
         <v>0.64</v>
       </c>
       <c r="D38">
@@ -1913,8 +1939,8 @@
       </c>
     </row>
     <row r="39" spans="6:7">
-      <c r="F39" s="20" t="s">
-        <v>35</v>
+      <c r="F39" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="G39">
         <f>SUM(G33:G38)</f>
@@ -1922,66 +1948,66 @@
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="24"/>
+      <c r="A40" s="25"/>
     </row>
     <row r="42" ht="15.75" spans="1:4">
       <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" spans="1:7">
+      <c r="A43" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" spans="1:7">
+      <c r="A44" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D42" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" spans="1:7">
-      <c r="A43" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D43" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" t="s">
-        <v>48</v>
-      </c>
-      <c r="G43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" spans="1:7">
-      <c r="A44" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>52</v>
-      </c>
       <c r="D44" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E44" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F44">
         <f>M24</f>
         <v>1</v>
       </c>
       <c r="G44" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" ht="15.75" spans="1:7">
-      <c r="A45" s="23">
+      <c r="A45" s="24">
         <v>1</v>
       </c>
-      <c r="B45" s="23">
+      <c r="B45" s="24">
         <v>10</v>
       </c>
-      <c r="C45" s="23">
+      <c r="C45" s="24">
         <v>1</v>
       </c>
       <c r="D45">
@@ -1998,13 +2024,13 @@
       </c>
     </row>
     <row r="46" ht="15.75" spans="1:7">
-      <c r="A46" s="23">
+      <c r="A46" s="24">
         <v>11</v>
       </c>
-      <c r="B46" s="23">
+      <c r="B46" s="24">
         <v>50</v>
       </c>
-      <c r="C46" s="23">
+      <c r="C46" s="24">
         <v>0.9</v>
       </c>
       <c r="D46">
@@ -2021,13 +2047,13 @@
       </c>
     </row>
     <row r="47" ht="15.75" spans="1:7">
-      <c r="A47" s="23">
+      <c r="A47" s="24">
         <v>51</v>
       </c>
-      <c r="B47" s="23">
+      <c r="B47" s="24">
         <v>100</v>
       </c>
-      <c r="C47" s="23">
+      <c r="C47" s="24">
         <v>0.85</v>
       </c>
       <c r="D47">
@@ -2044,13 +2070,13 @@
       </c>
     </row>
     <row r="48" ht="15.75" spans="1:7">
-      <c r="A48" s="23">
+      <c r="A48" s="24">
         <v>101</v>
       </c>
-      <c r="B48" s="23">
+      <c r="B48" s="24">
         <v>190</v>
       </c>
-      <c r="C48" s="23">
+      <c r="C48" s="24">
         <v>0.8</v>
       </c>
       <c r="D48">
@@ -2067,13 +2093,13 @@
       </c>
     </row>
     <row r="49" ht="15.75" spans="1:7">
-      <c r="A49" s="23">
+      <c r="A49" s="24">
         <v>191</v>
       </c>
-      <c r="B49" s="23">
+      <c r="B49" s="24">
         <v>2000</v>
       </c>
-      <c r="C49" s="23">
+      <c r="C49" s="24">
         <v>0.75</v>
       </c>
       <c r="D49">
@@ -2090,11 +2116,11 @@
       </c>
     </row>
     <row r="50" ht="15.75" spans="1:7">
-      <c r="A50" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23">
+      <c r="A50" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24">
         <v>0.69</v>
       </c>
       <c r="D50">
@@ -2111,8 +2137,8 @@
       </c>
     </row>
     <row r="51" spans="6:7">
-      <c r="F51" s="20" t="s">
-        <v>35</v>
+      <c r="F51" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="G51">
         <f>SUM(G45:G50)</f>
@@ -2120,7 +2146,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
+    <mergeCell ref="D7:E7"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="D14:E14"/>

</xml_diff>